<commit_message>
Updates Figure 9.27 with new corrigenda data
</commit_message>
<xml_diff>
--- a/Plotting_code_and_data/Fig9_27_SL_scenarios/Plot_Figure/AR6_GMSL_Models_v3.xlsx
+++ b/Plotting_code_and_data/Fig9_27_SL_scenarios/Plot_Figure/AR6_GMSL_Models_v3.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="14">
   <si>
     <t>Change in global mean sea level (GMSL) in meters compared to 1995-2014 average - FACTS Probabilistic Emulator Product</t>
   </si>
@@ -75,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="91">
     <border>
       <left/>
       <right/>
@@ -113,11 +113,71 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -149,6 +209,66 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,107 +314,107 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="11" t="s">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="23" t="s">
+      <c r="V1" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="87" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="21" t="s">
+      <c r="T2" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="25" t="s">
+      <c r="V2" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="25" t="s">
+      <c r="W2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="25" t="s">
+      <c r="X2" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" s="25" t="s">
+      <c r="Y2" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="29" t="s">
+      <c r="AA2" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="29" t="s">
+      <c r="AB2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="AC2" s="29" t="s">
+      <c r="AC2" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="AD2" s="29" t="s">
+      <c r="AD2" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="7" t="s">
+      <c r="AF2" s="67" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="65" t="s">
         <v>6</v>
       </c>
       <c r="G3">
@@ -357,19 +477,19 @@
       <c r="AD3">
         <v>0</v>
       </c>
-      <c r="AF3" s="9" t="s">
+      <c r="AF3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="AG3" s="9" t="s">
+      <c r="AG3" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AH3" s="9" t="s">
+      <c r="AH3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AI3" s="9" t="s">
+      <c r="AI3" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="AJ3" s="9" t="s">
+      <c r="AJ3" s="69" t="s">
         <v>6</v>
       </c>
     </row>
@@ -393,61 +513,61 @@
         <v>2020</v>
       </c>
       <c r="H4">
-        <v>0.050999999046325684</v>
+        <v>0.048999998718500137</v>
       </c>
       <c r="I4">
-        <v>0.045000001788139343</v>
+        <v>0.043000001460313797</v>
       </c>
       <c r="J4">
-        <v>0.063000001013278961</v>
+        <v>0.061000000685453415</v>
       </c>
       <c r="L4">
         <v>2020</v>
       </c>
       <c r="M4">
-        <v>0.050999999046325684</v>
+        <v>0.048999998718500137</v>
       </c>
       <c r="N4">
-        <v>0.045000001788139343</v>
+        <v>0.043000001460313797</v>
       </c>
       <c r="O4">
-        <v>0.063000001013278961</v>
+        <v>0.061000000685453415</v>
       </c>
       <c r="Q4">
         <v>2020</v>
       </c>
       <c r="R4">
-        <v>0.050999999046325684</v>
+        <v>0.048999998718500137</v>
       </c>
       <c r="S4">
-        <v>0.045000001788139343</v>
+        <v>0.043000001460313797</v>
       </c>
       <c r="T4">
-        <v>0.063000001013278961</v>
+        <v>0.061000000685453415</v>
       </c>
       <c r="V4">
         <v>2020</v>
       </c>
       <c r="W4">
-        <v>0.050999999046325684</v>
+        <v>0.048999998718500137</v>
       </c>
       <c r="X4">
-        <v>0.045000001788139343</v>
+        <v>0.043000001460313797</v>
       </c>
       <c r="Y4">
-        <v>0.063000001013278961</v>
+        <v>0.061000000685453415</v>
       </c>
       <c r="AA4">
         <v>2020</v>
       </c>
       <c r="AB4">
-        <v>0.050999999046325684</v>
+        <v>0.048999998718500137</v>
       </c>
       <c r="AC4">
-        <v>0.045000001788139343</v>
+        <v>0.043000001460313797</v>
       </c>
       <c r="AD4">
-        <v>0.063000001013278961</v>
+        <v>0.061000000685453415</v>
       </c>
       <c r="AF4">
         <v>2005</v>
@@ -470,91 +590,91 @@
         <v>2020</v>
       </c>
       <c r="B5">
-        <v>0.045000001788139343</v>
+        <v>0.043000001460313797</v>
       </c>
       <c r="C5">
-        <v>0.074000000953674316</v>
+        <v>0.071000002324581146</v>
       </c>
       <c r="D5">
-        <v>0.041000001132488251</v>
+        <v>0.039000000804662704</v>
       </c>
       <c r="E5">
-        <v>0.082999996840953827</v>
+        <v>0.081000000238418579</v>
       </c>
       <c r="G5">
         <v>2030</v>
       </c>
       <c r="H5">
-        <v>0.093999996781349182</v>
+        <v>0.092000000178813934</v>
       </c>
       <c r="I5">
-        <v>0.081000000238418579</v>
+        <v>0.079999998211860657</v>
       </c>
       <c r="J5">
-        <v>0.11800000071525574</v>
+        <v>0.11699999868869781</v>
       </c>
       <c r="L5">
         <v>2030</v>
       </c>
       <c r="M5">
-        <v>0.093999996781349182</v>
+        <v>0.092000000178813934</v>
       </c>
       <c r="N5">
-        <v>0.081000000238418579</v>
+        <v>0.079999998211860657</v>
       </c>
       <c r="O5">
-        <v>0.11800000071525574</v>
+        <v>0.11699999868869781</v>
       </c>
       <c r="Q5">
         <v>2030</v>
       </c>
       <c r="R5">
-        <v>0.093999996781349182</v>
+        <v>0.092000000178813934</v>
       </c>
       <c r="S5">
-        <v>0.081000000238418579</v>
+        <v>0.079999998211860657</v>
       </c>
       <c r="T5">
-        <v>0.11800000071525574</v>
+        <v>0.11699999868869781</v>
       </c>
       <c r="V5">
         <v>2030</v>
       </c>
       <c r="W5">
-        <v>0.093999996781349182</v>
+        <v>0.092000000178813934</v>
       </c>
       <c r="X5">
-        <v>0.081000000238418579</v>
+        <v>0.079999998211860657</v>
       </c>
       <c r="Y5">
-        <v>0.11800000071525574</v>
+        <v>0.11699999868869781</v>
       </c>
       <c r="AA5">
         <v>2030</v>
       </c>
       <c r="AB5">
-        <v>0.093999996781349182</v>
+        <v>0.092000000178813934</v>
       </c>
       <c r="AC5">
-        <v>0.081000000238418579</v>
+        <v>0.079999998211860657</v>
       </c>
       <c r="AD5">
-        <v>0.11800000071525574</v>
+        <v>0.11699999868869781</v>
       </c>
       <c r="AF5">
         <v>2020</v>
       </c>
       <c r="AG5">
-        <v>0.045000001788139343</v>
+        <v>0.043000001460313797</v>
       </c>
       <c r="AH5">
-        <v>0.071999996900558472</v>
+        <v>0.070000000298023224</v>
       </c>
       <c r="AI5">
-        <v>0.041000001132488251</v>
+        <v>0.039000000804662704</v>
       </c>
       <c r="AJ5">
-        <v>0.079000003635883331</v>
+        <v>0.076999999582767487</v>
       </c>
     </row>
     <row r="6">
@@ -562,91 +682,91 @@
         <v>2030</v>
       </c>
       <c r="B6">
-        <v>0.086999997496604919</v>
+        <v>0.085000000894069672</v>
       </c>
       <c r="C6">
-        <v>0.15199999511241913</v>
+        <v>0.15000000596046448</v>
       </c>
       <c r="D6">
-        <v>0.075999997556209564</v>
+        <v>0.074000000953674316</v>
       </c>
       <c r="E6">
-        <v>0.19699999690055847</v>
+        <v>0.19499999284744263</v>
       </c>
       <c r="G6">
         <v>2040</v>
       </c>
       <c r="H6">
-        <v>0.12999999523162842</v>
+        <v>0.12800000607967377</v>
       </c>
       <c r="I6">
-        <v>0.10899999737739563</v>
+        <v>0.10700000077486038</v>
       </c>
       <c r="J6">
-        <v>0.16899999976158142</v>
+        <v>0.1679999977350235</v>
       </c>
       <c r="L6">
         <v>2040</v>
       </c>
       <c r="M6">
-        <v>0.12999999523162842</v>
+        <v>0.12800000607967377</v>
       </c>
       <c r="N6">
-        <v>0.10899999737739563</v>
+        <v>0.10700000077486038</v>
       </c>
       <c r="O6">
-        <v>0.16899999976158142</v>
+        <v>0.1679999977350235</v>
       </c>
       <c r="Q6">
         <v>2040</v>
       </c>
       <c r="R6">
-        <v>0.12999999523162842</v>
+        <v>0.12800000607967377</v>
       </c>
       <c r="S6">
-        <v>0.10899999737739563</v>
+        <v>0.10700000077486038</v>
       </c>
       <c r="T6">
-        <v>0.16899999976158142</v>
+        <v>0.1679999977350235</v>
       </c>
       <c r="V6">
         <v>2040</v>
       </c>
       <c r="W6">
-        <v>0.12999999523162842</v>
+        <v>0.12800000607967377</v>
       </c>
       <c r="X6">
-        <v>0.10899999737739563</v>
+        <v>0.10700000077486038</v>
       </c>
       <c r="Y6">
-        <v>0.16899999976158142</v>
+        <v>0.1679999977350235</v>
       </c>
       <c r="AA6">
         <v>2040</v>
       </c>
       <c r="AB6">
-        <v>0.12999999523162842</v>
+        <v>0.12800000607967377</v>
       </c>
       <c r="AC6">
-        <v>0.10899999737739563</v>
+        <v>0.10700000077486038</v>
       </c>
       <c r="AD6">
-        <v>0.16899999976158142</v>
+        <v>0.1679999977350235</v>
       </c>
       <c r="AF6">
         <v>2030</v>
       </c>
       <c r="AG6">
-        <v>0.082000002264976501</v>
+        <v>0.079000003635883331</v>
       </c>
       <c r="AH6">
-        <v>0.14000000059604645</v>
+        <v>0.1379999965429306</v>
       </c>
       <c r="AI6">
-        <v>0.074000000953674316</v>
+        <v>0.071999996900558472</v>
       </c>
       <c r="AJ6">
-        <v>0.17100000381469727</v>
+        <v>0.16899999976158142</v>
       </c>
     </row>
     <row r="7">
@@ -654,91 +774,91 @@
         <v>2040</v>
       </c>
       <c r="B7">
-        <v>0.13500000536441803</v>
+        <v>0.13300000131130219</v>
       </c>
       <c r="C7">
-        <v>0.25999999046325684</v>
+        <v>0.25799998641014099</v>
       </c>
       <c r="D7">
-        <v>0.11100000143051147</v>
+        <v>0.1080000028014183</v>
       </c>
       <c r="E7">
-        <v>0.35499998927116394</v>
+        <v>0.35199999809265137</v>
       </c>
       <c r="G7">
         <v>2050</v>
       </c>
       <c r="H7">
-        <v>0.17800000309944153</v>
+        <v>0.17599999904632568</v>
       </c>
       <c r="I7">
-        <v>0.14800000190734863</v>
+        <v>0.14599999785423279</v>
       </c>
       <c r="J7">
-        <v>0.23399999737739563</v>
+        <v>0.23199999332427979</v>
       </c>
       <c r="L7">
         <v>2050</v>
       </c>
       <c r="M7">
-        <v>0.17800000309944153</v>
+        <v>0.17599999904632568</v>
       </c>
       <c r="N7">
-        <v>0.14800000190734863</v>
+        <v>0.14599999785423279</v>
       </c>
       <c r="O7">
-        <v>0.23399999737739563</v>
+        <v>0.23199999332427979</v>
       </c>
       <c r="Q7">
         <v>2050</v>
       </c>
       <c r="R7">
-        <v>0.17800000309944153</v>
+        <v>0.17599999904632568</v>
       </c>
       <c r="S7">
-        <v>0.14800000190734863</v>
+        <v>0.14599999785423279</v>
       </c>
       <c r="T7">
-        <v>0.23399999737739563</v>
+        <v>0.23199999332427979</v>
       </c>
       <c r="V7">
         <v>2050</v>
       </c>
       <c r="W7">
-        <v>0.17800000309944153</v>
+        <v>0.17599999904632568</v>
       </c>
       <c r="X7">
-        <v>0.14800000190734863</v>
+        <v>0.14599999785423279</v>
       </c>
       <c r="Y7">
-        <v>0.23399999737739563</v>
+        <v>0.23199999332427979</v>
       </c>
       <c r="AA7">
         <v>2050</v>
       </c>
       <c r="AB7">
-        <v>0.17800000309944153</v>
+        <v>0.17599999904632568</v>
       </c>
       <c r="AC7">
-        <v>0.14800000190734863</v>
+        <v>0.14599999785423279</v>
       </c>
       <c r="AD7">
-        <v>0.23399999737739563</v>
+        <v>0.23199999332427979</v>
       </c>
       <c r="AF7">
         <v>2040</v>
       </c>
       <c r="AG7">
-        <v>0.11599999666213989</v>
+        <v>0.11400000005960464</v>
       </c>
       <c r="AH7">
-        <v>0.22300000488758087</v>
+        <v>0.22100000083446503</v>
       </c>
       <c r="AI7">
-        <v>0.10300000011920929</v>
+        <v>0.10000000149011612</v>
       </c>
       <c r="AJ7">
-        <v>0.28499999642372131</v>
+        <v>0.28200000524520874</v>
       </c>
     </row>
     <row r="8">
@@ -746,91 +866,91 @@
         <v>2050</v>
       </c>
       <c r="B8">
-        <v>0.19799999892711639</v>
+        <v>0.19499999284744263</v>
       </c>
       <c r="C8">
-        <v>0.40000000596046448</v>
+        <v>0.3970000147819519</v>
       </c>
       <c r="D8">
-        <v>0.164000004529953</v>
+        <v>0.15899999439716339</v>
       </c>
       <c r="E8">
-        <v>0.5429999828338623</v>
+        <v>0.54100000858306885</v>
       </c>
       <c r="G8">
         <v>2060</v>
       </c>
       <c r="H8">
-        <v>0.21199999749660492</v>
+        <v>0.20999999344348907</v>
       </c>
       <c r="I8">
-        <v>0.17200000584125519</v>
+        <v>0.16899999976158142</v>
       </c>
       <c r="J8">
-        <v>0.28799998760223389</v>
+        <v>0.28600001335144043</v>
       </c>
       <c r="L8">
         <v>2060</v>
       </c>
       <c r="M8">
-        <v>0.21199999749660492</v>
+        <v>0.20999999344348907</v>
       </c>
       <c r="N8">
-        <v>0.17200000584125519</v>
+        <v>0.16899999976158142</v>
       </c>
       <c r="O8">
-        <v>0.28799998760223389</v>
+        <v>0.28600001335144043</v>
       </c>
       <c r="Q8">
         <v>2060</v>
       </c>
       <c r="R8">
-        <v>0.21199999749660492</v>
+        <v>0.20999999344348907</v>
       </c>
       <c r="S8">
-        <v>0.17200000584125519</v>
+        <v>0.16899999976158142</v>
       </c>
       <c r="T8">
-        <v>0.28799998760223389</v>
+        <v>0.28600001335144043</v>
       </c>
       <c r="V8">
         <v>2060</v>
       </c>
       <c r="W8">
-        <v>0.21199999749660492</v>
+        <v>0.20999999344348907</v>
       </c>
       <c r="X8">
-        <v>0.17200000584125519</v>
+        <v>0.16899999976158142</v>
       </c>
       <c r="Y8">
-        <v>0.28799998760223389</v>
+        <v>0.28600001335144043</v>
       </c>
       <c r="AA8">
         <v>2060</v>
       </c>
       <c r="AB8">
-        <v>0.21199999749660492</v>
+        <v>0.20999999344348907</v>
       </c>
       <c r="AC8">
-        <v>0.17200000584125519</v>
+        <v>0.16899999976158142</v>
       </c>
       <c r="AD8">
-        <v>0.28799998760223389</v>
+        <v>0.28600001335144043</v>
       </c>
       <c r="AF8">
         <v>2050</v>
       </c>
       <c r="AG8">
-        <v>0.15999999642372131</v>
+        <v>0.15800000727176666</v>
       </c>
       <c r="AH8">
-        <v>0.31299999356269836</v>
+        <v>0.31000000238418579</v>
       </c>
       <c r="AI8">
-        <v>0.13400000333786011</v>
+        <v>0.12999999523162842</v>
       </c>
       <c r="AJ8">
-        <v>0.40299999713897705</v>
+        <v>0.40000000596046448</v>
       </c>
     </row>
     <row r="9">
@@ -838,91 +958,91 @@
         <v>2060</v>
       </c>
       <c r="B9">
-        <v>0.26199999451637268</v>
+        <v>0.25900000333786011</v>
       </c>
       <c r="C9">
-        <v>0.57200002670288086</v>
+        <v>0.5690000057220459</v>
       </c>
       <c r="D9">
-        <v>0.23000000417232513</v>
+        <v>0.22400000691413879</v>
       </c>
       <c r="E9">
-        <v>0.76899999380111694</v>
+        <v>0.76700001955032349</v>
       </c>
       <c r="G9">
         <v>2070</v>
       </c>
       <c r="H9">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="I9">
-        <v>0.20800000429153442</v>
+        <v>0.20600000023841858</v>
       </c>
       <c r="J9">
-        <v>0.35899999737739563</v>
+        <v>0.35600000619888306</v>
       </c>
       <c r="L9">
         <v>2070</v>
       </c>
       <c r="M9">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="N9">
-        <v>0.20800000429153442</v>
+        <v>0.20600000023841858</v>
       </c>
       <c r="O9">
-        <v>0.35899999737739563</v>
+        <v>0.35600000619888306</v>
       </c>
       <c r="Q9">
         <v>2070</v>
       </c>
       <c r="R9">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="S9">
-        <v>0.20800000429153442</v>
+        <v>0.20600000023841858</v>
       </c>
       <c r="T9">
-        <v>0.35899999737739563</v>
+        <v>0.35600000619888306</v>
       </c>
       <c r="V9">
         <v>2070</v>
       </c>
       <c r="W9">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="X9">
-        <v>0.20800000429153442</v>
+        <v>0.20600000023841858</v>
       </c>
       <c r="Y9">
-        <v>0.35899999737739563</v>
+        <v>0.35600000619888306</v>
       </c>
       <c r="AA9">
         <v>2070</v>
       </c>
       <c r="AB9">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="AC9">
-        <v>0.20800000429153442</v>
+        <v>0.20600000023841858</v>
       </c>
       <c r="AD9">
-        <v>0.35899999737739563</v>
+        <v>0.35600000619888306</v>
       </c>
       <c r="AF9">
         <v>2060</v>
       </c>
       <c r="AG9">
-        <v>0.19300000369548798</v>
+        <v>0.19200000166893005</v>
       </c>
       <c r="AH9">
-        <v>0.40200001001358032</v>
+        <v>0.39899998903274536</v>
       </c>
       <c r="AI9">
-        <v>0.1679999977350235</v>
+        <v>0.164000004529953</v>
       </c>
       <c r="AJ9">
-        <v>0.51800000667572021</v>
+        <v>0.51599997282028198</v>
       </c>
     </row>
     <row r="10">
@@ -930,91 +1050,91 @@
         <v>2070</v>
       </c>
       <c r="B10">
-        <v>0.34099999070167542</v>
+        <v>0.33899998664855957</v>
       </c>
       <c r="C10">
-        <v>0.7839999794960022</v>
+        <v>0.77799999713897705</v>
       </c>
       <c r="D10">
-        <v>0.30399999022483826</v>
+        <v>0.29600000381469727</v>
       </c>
       <c r="E10">
-        <v>1.0479999780654907</v>
+        <v>1.0460000038146973</v>
       </c>
       <c r="G10">
         <v>2080</v>
       </c>
       <c r="H10">
-        <v>0.30300000309944153</v>
+        <v>0.30099999904632568</v>
       </c>
       <c r="I10">
-        <v>0.23199999332427979</v>
+        <v>0.23100000619888306</v>
       </c>
       <c r="J10">
-        <v>0.42199999094009399</v>
+        <v>0.42100000381469727</v>
       </c>
       <c r="L10">
         <v>2080</v>
       </c>
       <c r="M10">
-        <v>0.30300000309944153</v>
+        <v>0.30099999904632568</v>
       </c>
       <c r="N10">
-        <v>0.23199999332427979</v>
+        <v>0.23100000619888306</v>
       </c>
       <c r="O10">
-        <v>0.42199999094009399</v>
+        <v>0.42100000381469727</v>
       </c>
       <c r="Q10">
         <v>2080</v>
       </c>
       <c r="R10">
-        <v>0.30300000309944153</v>
+        <v>0.30099999904632568</v>
       </c>
       <c r="S10">
-        <v>0.23199999332427979</v>
+        <v>0.23100000619888306</v>
       </c>
       <c r="T10">
-        <v>0.42199999094009399</v>
+        <v>0.42100000381469727</v>
       </c>
       <c r="V10">
         <v>2080</v>
       </c>
       <c r="W10">
-        <v>0.30300000309944153</v>
+        <v>0.30099999904632568</v>
       </c>
       <c r="X10">
-        <v>0.23199999332427979</v>
+        <v>0.23100000619888306</v>
       </c>
       <c r="Y10">
-        <v>0.42199999094009399</v>
+        <v>0.42100000381469727</v>
       </c>
       <c r="AA10">
         <v>2080</v>
       </c>
       <c r="AB10">
-        <v>0.30300000309944153</v>
+        <v>0.30099999904632568</v>
       </c>
       <c r="AC10">
-        <v>0.23199999332427979</v>
+        <v>0.23100000619888306</v>
       </c>
       <c r="AD10">
-        <v>0.42199999094009399</v>
+        <v>0.42100000381469727</v>
       </c>
       <c r="AF10">
         <v>2070</v>
       </c>
       <c r="AG10">
-        <v>0.23600000143051147</v>
+        <v>0.23399999737739563</v>
       </c>
       <c r="AH10">
-        <v>0.49399998784065247</v>
+        <v>0.49000000953674316</v>
       </c>
       <c r="AI10">
-        <v>0.20299999415874481</v>
+        <v>0.19799999892711639</v>
       </c>
       <c r="AJ10">
-        <v>0.64399999380111694</v>
+        <v>0.6380000114440918</v>
       </c>
     </row>
     <row r="11">
@@ -1022,91 +1142,91 @@
         <v>2080</v>
       </c>
       <c r="B11">
-        <v>0.42399999499320984</v>
+        <v>0.41999998688697815</v>
       </c>
       <c r="C11">
-        <v>1.0360000133514404</v>
+        <v>1.0279999971389771</v>
       </c>
       <c r="D11">
-        <v>0.38100001215934753</v>
+        <v>0.37200000882148743</v>
       </c>
       <c r="E11">
-        <v>1.3999999761581421</v>
+        <v>1.3980000019073486</v>
       </c>
       <c r="G11">
         <v>2090</v>
       </c>
       <c r="H11">
-        <v>0.34999999403953552</v>
+        <v>0.34700000286102295</v>
       </c>
       <c r="I11">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="J11">
-        <v>0.49000000953674316</v>
+        <v>0.48899999260902405</v>
       </c>
       <c r="L11">
         <v>2090</v>
       </c>
       <c r="M11">
-        <v>0.34999999403953552</v>
+        <v>0.34700000286102295</v>
       </c>
       <c r="N11">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="O11">
-        <v>0.49000000953674316</v>
+        <v>0.48899999260902405</v>
       </c>
       <c r="Q11">
         <v>2090</v>
       </c>
       <c r="R11">
-        <v>0.34999999403953552</v>
+        <v>0.34700000286102295</v>
       </c>
       <c r="S11">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="T11">
-        <v>0.49000000953674316</v>
+        <v>0.48899999260902405</v>
       </c>
       <c r="V11">
         <v>2090</v>
       </c>
       <c r="W11">
-        <v>0.34999999403953552</v>
+        <v>0.34700000286102295</v>
       </c>
       <c r="X11">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="Y11">
-        <v>0.49000000953674316</v>
+        <v>0.48899999260902405</v>
       </c>
       <c r="AA11">
         <v>2090</v>
       </c>
       <c r="AB11">
-        <v>0.34999999403953552</v>
+        <v>0.34700000286102295</v>
       </c>
       <c r="AC11">
-        <v>0.26199999451637268</v>
+        <v>0.25999999046325684</v>
       </c>
       <c r="AD11">
-        <v>0.49000000953674316</v>
+        <v>0.48899999260902405</v>
       </c>
       <c r="AF11">
         <v>2080</v>
       </c>
       <c r="AG11">
-        <v>0.26800000667572021</v>
+        <v>0.26600000262260437</v>
       </c>
       <c r="AH11">
-        <v>0.5899999737739563</v>
+        <v>0.58499997854232788</v>
       </c>
       <c r="AI11">
-        <v>0.23000000417232513</v>
+        <v>0.22900000214576721</v>
       </c>
       <c r="AJ11">
-        <v>0.77799999713897705</v>
+        <v>0.77499997615814209</v>
       </c>
     </row>
     <row r="12">
@@ -1114,91 +1234,91 @@
         <v>2090</v>
       </c>
       <c r="B12">
-        <v>0.52499997615814209</v>
+        <v>0.51999998092651367</v>
       </c>
       <c r="C12">
-        <v>1.3090000152587891</v>
+        <v>1.3040000200271606</v>
       </c>
       <c r="D12">
-        <v>0.460999995470047</v>
+        <v>0.44999998807907104</v>
       </c>
       <c r="E12">
-        <v>1.8059999942779541</v>
+        <v>1.7999999523162842</v>
       </c>
       <c r="G12">
         <v>2100</v>
       </c>
       <c r="H12">
-        <v>0.38499999046325684</v>
+        <v>0.38400000333786011</v>
       </c>
       <c r="I12">
-        <v>0.27599999308586121</v>
+        <v>0.27500000596046448</v>
       </c>
       <c r="J12">
-        <v>0.54900002479553223</v>
+        <v>0.54799997806549072</v>
       </c>
       <c r="L12">
         <v>2100</v>
       </c>
       <c r="M12">
-        <v>0.38499999046325684</v>
+        <v>0.38400000333786011</v>
       </c>
       <c r="N12">
-        <v>0.27599999308586121</v>
+        <v>0.27500000596046448</v>
       </c>
       <c r="O12">
-        <v>0.54900002479553223</v>
+        <v>0.54799997806549072</v>
       </c>
       <c r="Q12">
         <v>2100</v>
       </c>
       <c r="R12">
-        <v>0.38499999046325684</v>
+        <v>0.38400000333786011</v>
       </c>
       <c r="S12">
-        <v>0.27599999308586121</v>
+        <v>0.27500000596046448</v>
       </c>
       <c r="T12">
-        <v>0.54900002479553223</v>
+        <v>0.54799997806549072</v>
       </c>
       <c r="V12">
         <v>2100</v>
       </c>
       <c r="W12">
-        <v>0.38499999046325684</v>
+        <v>0.38400000333786011</v>
       </c>
       <c r="X12">
-        <v>0.27599999308586121</v>
+        <v>0.27500000596046448</v>
       </c>
       <c r="Y12">
-        <v>0.54900002479553223</v>
+        <v>0.54799997806549072</v>
       </c>
       <c r="AA12">
         <v>2100</v>
       </c>
       <c r="AB12">
-        <v>0.38499999046325684</v>
+        <v>0.38400000333786011</v>
       </c>
       <c r="AC12">
-        <v>0.27599999308586121</v>
+        <v>0.27500000596046448</v>
       </c>
       <c r="AD12">
-        <v>0.54900002479553223</v>
+        <v>0.54799997806549072</v>
       </c>
       <c r="AF12">
         <v>2090</v>
       </c>
       <c r="AG12">
-        <v>0.29899999499320984</v>
+        <v>0.29800000786781311</v>
       </c>
       <c r="AH12">
-        <v>0.68800002336502075</v>
+        <v>0.68400001525878906</v>
       </c>
       <c r="AI12">
-        <v>0.25299999117851257</v>
+        <v>0.25200000405311584</v>
       </c>
       <c r="AJ12">
-        <v>0.93000000715255737</v>
+        <v>0.92500001192092896</v>
       </c>
     </row>
     <row r="13">
@@ -1206,91 +1326,91 @@
         <v>2100</v>
       </c>
       <c r="B13">
-        <v>0.63099998235702515</v>
+        <v>0.625</v>
       </c>
       <c r="C13">
-        <v>1.6080000400543213</v>
+        <v>1.6030000448226929</v>
       </c>
       <c r="D13">
-        <v>0.54000002145767212</v>
+        <v>0.52999997138977051</v>
       </c>
       <c r="E13">
-        <v>2.2799999713897705</v>
+        <v>2.2739999294281006</v>
       </c>
       <c r="G13">
         <v>2130</v>
       </c>
       <c r="H13">
-        <v>0.50599998235702515</v>
+        <v>0.50099998712539673</v>
       </c>
       <c r="I13">
-        <v>0.34099999070167542</v>
+        <v>0.33500000834465027</v>
       </c>
       <c r="J13">
-        <v>0.74099999666213989</v>
+        <v>0.74000000953674316</v>
       </c>
       <c r="L13">
         <v>2130</v>
       </c>
       <c r="M13">
-        <v>0.50599998235702515</v>
+        <v>0.50099998712539673</v>
       </c>
       <c r="N13">
-        <v>0.34099999070167542</v>
+        <v>0.33500000834465027</v>
       </c>
       <c r="O13">
-        <v>0.74099999666213989</v>
+        <v>0.74000000953674316</v>
       </c>
       <c r="Q13">
         <v>2130</v>
       </c>
       <c r="R13">
-        <v>0.50599998235702515</v>
+        <v>0.50099998712539673</v>
       </c>
       <c r="S13">
-        <v>0.34099999070167542</v>
+        <v>0.33500000834465027</v>
       </c>
       <c r="T13">
-        <v>0.74099999666213989</v>
+        <v>0.74000000953674316</v>
       </c>
       <c r="V13">
         <v>2130</v>
       </c>
       <c r="W13">
-        <v>0.50599998235702515</v>
+        <v>0.50099998712539673</v>
       </c>
       <c r="X13">
-        <v>0.34099999070167542</v>
+        <v>0.33500000834465027</v>
       </c>
       <c r="Y13">
-        <v>0.74099999666213989</v>
+        <v>0.74000000953674316</v>
       </c>
       <c r="AA13">
         <v>2130</v>
       </c>
       <c r="AB13">
-        <v>0.50599998235702515</v>
+        <v>0.50099998712539673</v>
       </c>
       <c r="AC13">
-        <v>0.34099999070167542</v>
+        <v>0.33500000834465027</v>
       </c>
       <c r="AD13">
-        <v>0.74099999666213989</v>
+        <v>0.74000000953674316</v>
       </c>
       <c r="AF13">
         <v>2100</v>
       </c>
       <c r="AG13">
-        <v>0.32600000500679016</v>
+        <v>0.32400000095367432</v>
       </c>
       <c r="AH13">
-        <v>0.79500001668930054</v>
+        <v>0.79100000858306885</v>
       </c>
       <c r="AI13">
-        <v>0.26399999856948853</v>
+        <v>0.26499998569488525</v>
       </c>
       <c r="AJ13">
-        <v>1.0880000591278076</v>
+        <v>1.0850000381469727</v>
       </c>
     </row>
     <row r="14">
@@ -1298,91 +1418,91 @@
         <v>2130</v>
       </c>
       <c r="B14">
-        <v>0.84500002861022949</v>
+        <v>0.81800001859664917</v>
       </c>
       <c r="C14">
-        <v>2.8559999465942383</v>
+        <v>2.8480000495910645</v>
       </c>
       <c r="D14">
-        <v>0.73600000143051147</v>
+        <v>0.70599997043609619</v>
       </c>
       <c r="E14">
-        <v>4.0590000152587891</v>
+        <v>4.0489997863769531</v>
       </c>
       <c r="G14">
         <v>2140</v>
       </c>
       <c r="H14">
-        <v>0.54000002145767212</v>
+        <v>0.5350000262260437</v>
       </c>
       <c r="I14">
-        <v>0.3580000102519989</v>
+        <v>0.3529999852180481</v>
       </c>
       <c r="J14">
-        <v>0.79900002479553223</v>
+        <v>0.79799997806549072</v>
       </c>
       <c r="L14">
         <v>2140</v>
       </c>
       <c r="M14">
-        <v>0.54000002145767212</v>
+        <v>0.5350000262260437</v>
       </c>
       <c r="N14">
-        <v>0.3580000102519989</v>
+        <v>0.3529999852180481</v>
       </c>
       <c r="O14">
-        <v>0.79900002479553223</v>
+        <v>0.79799997806549072</v>
       </c>
       <c r="Q14">
         <v>2140</v>
       </c>
       <c r="R14">
-        <v>0.54000002145767212</v>
+        <v>0.5350000262260437</v>
       </c>
       <c r="S14">
-        <v>0.3580000102519989</v>
+        <v>0.3529999852180481</v>
       </c>
       <c r="T14">
-        <v>0.79900002479553223</v>
+        <v>0.79799997806549072</v>
       </c>
       <c r="V14">
         <v>2140</v>
       </c>
       <c r="W14">
-        <v>0.54000002145767212</v>
+        <v>0.5350000262260437</v>
       </c>
       <c r="X14">
-        <v>0.3580000102519989</v>
+        <v>0.3529999852180481</v>
       </c>
       <c r="Y14">
-        <v>0.79900002479553223</v>
+        <v>0.79799997806549072</v>
       </c>
       <c r="AA14">
         <v>2140</v>
       </c>
       <c r="AB14">
-        <v>0.54000002145767212</v>
+        <v>0.5350000262260437</v>
       </c>
       <c r="AC14">
-        <v>0.3580000102519989</v>
+        <v>0.3529999852180481</v>
       </c>
       <c r="AD14">
-        <v>0.79900002479553223</v>
+        <v>0.79799997806549072</v>
       </c>
       <c r="AF14">
         <v>2130</v>
       </c>
       <c r="AG14">
-        <v>0.414000004529953</v>
+        <v>0.40700000524520874</v>
       </c>
       <c r="AH14">
-        <v>1.121999979019165</v>
+        <v>1.1169999837875366</v>
       </c>
       <c r="AI14">
-        <v>0.34400001168251038</v>
+        <v>0.33500000834465027</v>
       </c>
       <c r="AJ14">
-        <v>1.5640000104904175</v>
+        <v>1.5529999732971191</v>
       </c>
     </row>
     <row r="15">
@@ -1390,91 +1510,91 @@
         <v>2140</v>
       </c>
       <c r="B15">
-        <v>0.93400001525878906</v>
+        <v>0.89999997615814209</v>
       </c>
       <c r="C15">
-        <v>3.8050000667572021</v>
+        <v>3.7969999313354492</v>
       </c>
       <c r="D15">
-        <v>0.81199997663497925</v>
+        <v>0.77600002288818359</v>
       </c>
       <c r="E15">
-        <v>4.7379999160766602</v>
+        <v>4.7410001754760742</v>
       </c>
       <c r="G15">
         <v>2150</v>
       </c>
       <c r="H15">
-        <v>0.57200002670288086</v>
+        <v>0.5690000057220459</v>
       </c>
       <c r="I15">
-        <v>0.37400001287460327</v>
+        <v>0.36899998784065247</v>
       </c>
       <c r="J15">
-        <v>0.8529999852180481</v>
+        <v>0.85500001907348633</v>
       </c>
       <c r="L15">
         <v>2150</v>
       </c>
       <c r="M15">
-        <v>0.57200002670288086</v>
+        <v>0.5690000057220459</v>
       </c>
       <c r="N15">
-        <v>0.37400001287460327</v>
+        <v>0.36899998784065247</v>
       </c>
       <c r="O15">
-        <v>0.8529999852180481</v>
+        <v>0.85500001907348633</v>
       </c>
       <c r="Q15">
         <v>2150</v>
       </c>
       <c r="R15">
-        <v>0.57200002670288086</v>
+        <v>0.5690000057220459</v>
       </c>
       <c r="S15">
-        <v>0.37400001287460327</v>
+        <v>0.36899998784065247</v>
       </c>
       <c r="T15">
-        <v>0.8529999852180481</v>
+        <v>0.85500001907348633</v>
       </c>
       <c r="V15">
         <v>2150</v>
       </c>
       <c r="W15">
-        <v>0.57200002670288086</v>
+        <v>0.5690000057220459</v>
       </c>
       <c r="X15">
-        <v>0.37400001287460327</v>
+        <v>0.36899998784065247</v>
       </c>
       <c r="Y15">
-        <v>0.8529999852180481</v>
+        <v>0.85500001907348633</v>
       </c>
       <c r="AA15">
         <v>2150</v>
       </c>
       <c r="AB15">
-        <v>0.57200002670288086</v>
+        <v>0.5690000057220459</v>
       </c>
       <c r="AC15">
-        <v>0.37400001287460327</v>
+        <v>0.36899998784065247</v>
       </c>
       <c r="AD15">
-        <v>0.8529999852180481</v>
+        <v>0.85500001907348633</v>
       </c>
       <c r="AF15">
         <v>2140</v>
       </c>
       <c r="AG15">
-        <v>0.43999999761581421</v>
+        <v>0.43299999833106995</v>
       </c>
       <c r="AH15">
-        <v>1.2319999933242798</v>
+        <v>1.2259999513626099</v>
       </c>
       <c r="AI15">
-        <v>0.36300000548362732</v>
+        <v>0.35400000214576721</v>
       </c>
       <c r="AJ15">
-        <v>1.718000054359436</v>
+        <v>1.7089999914169312</v>
       </c>
     </row>
     <row r="16">
@@ -1482,31 +1602,31 @@
         <v>2150</v>
       </c>
       <c r="B16">
-        <v>1.0160000324249268</v>
+        <v>0.97600001096725464</v>
       </c>
       <c r="C16">
-        <v>4.8289999961853027</v>
+        <v>4.8210000991821289</v>
       </c>
       <c r="D16">
-        <v>0.88499999046325684</v>
+        <v>0.83899998664855957</v>
       </c>
       <c r="E16">
-        <v>5.440000057220459</v>
+        <v>5.434999942779541</v>
       </c>
       <c r="AF16">
         <v>2150</v>
       </c>
       <c r="AG16">
-        <v>0.46399998664855957</v>
+        <v>0.45699998736381531</v>
       </c>
       <c r="AH16">
-        <v>1.343999981880188</v>
+        <v>1.3370000123977661</v>
       </c>
       <c r="AI16">
-        <v>0.37999999523162842</v>
+        <v>0.37099999189376831</v>
       </c>
       <c r="AJ16">
-        <v>1.8769999742507935</v>
+        <v>1.8739999532699585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>